<commit_message>
update sim input and fix one error
</commit_message>
<xml_diff>
--- a/Data/Sampling_input.xlsx
+++ b/Data/Sampling_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mysite.volvocars.net/personal/xyang118_volvocars_com/Documents/Documents/glance_simulation/sim1/Glance_sampling/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XYANG118\OneDrive - Volvo Cars\Documents\glance_simulation\sim3\Glance_sampling\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{4AF0046C-C6EE-403D-851D-C86931F82143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{926C75E2-3048-47E2-B162-077D803435BB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9AFC45-32A6-46BB-A661-F697B78638F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>sim_order</t>
   </si>
@@ -54,37 +54,40 @@
     <t>use_logic</t>
   </si>
   <si>
-    <t>optimised</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>baseline impact speed distribution</t>
-  </si>
-  <si>
     <t>impact speed reduction</t>
   </si>
   <si>
     <t>crash avoidance</t>
   </si>
   <si>
-    <t>injury risk reduction</t>
-  </si>
-  <si>
-    <t>SRS</t>
-  </si>
-  <si>
     <t>importance sampling</t>
   </si>
   <si>
-    <t>pps, size = prior weight</t>
-  </si>
-  <si>
-    <t>pps, size = prior weight * severity</t>
-  </si>
-  <si>
-    <t>all</t>
+    <t>opt_method</t>
+  </si>
+  <si>
+    <t>simple random sampling</t>
+  </si>
+  <si>
+    <t>active sampling</t>
+  </si>
+  <si>
+    <t>density sampling</t>
+  </si>
+  <si>
+    <t>severity sampling</t>
+  </si>
+  <si>
+    <t>naive</t>
+  </si>
+  <si>
+    <t>prediction uncertainty</t>
+  </si>
+  <si>
+    <t>model uncertainty</t>
   </si>
 </sst>
 </file>
@@ -120,13 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,23 +443,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK11"/>
+  <dimension ref="A1:AML12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="1" customWidth="1"/>
     <col min="3" max="3" width="45.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="50.109375" style="1" customWidth="1"/>
-    <col min="6" max="1025" width="8.88671875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="31.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.109375" style="1" customWidth="1"/>
+    <col min="7" max="1026" width="8.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -471,221 +473,236 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>12</v>
       </c>
-      <c r="F7" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="B10" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="G10" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>